<commit_message>
Send total_detected_objects to specfic excel cell automation
</commit_message>
<xml_diff>
--- a/ObjectDetection/ObjectDectecionWithOpenCV/test.xlsx
+++ b/ObjectDetection/ObjectDectecionWithOpenCV/test.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -362,15 +364,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>31</v>
       </c>
@@ -378,12 +380,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>31</v>
       </c>
@@ -391,17 +393,20 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I7">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>31</v>
       </c>
@@ -413,14 +418,73 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="10" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <v>38</v>
+      </c>
+      <c r="I6">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Rearranged Code and Rename Variable, Function With Coding Standards
</commit_message>
<xml_diff>
--- a/ObjectDetection/ObjectDectecionWithOpenCV/test.xlsx
+++ b/ObjectDetection/ObjectDectecionWithOpenCV/test.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -418,15 +419,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="10" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D10">
         <v>38</v>
       </c>
@@ -437,6 +448,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>31</v>
+      </c>
+      <c r="B1">
+        <v>53</v>
+      </c>
+      <c r="C1">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:I9"/>
   <sheetViews>
@@ -469,19 +506,34 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E4"/>
+  <dimension ref="B3:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E4">
         <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>